<commit_message>
Upload new version with timestamp
</commit_message>
<xml_diff>
--- a/DMSNewVSale_2025-09-17.xlsx
+++ b/DMSNewVSale_2025-09-17.xlsx
@@ -41,58 +41,7 @@
     <t>عدد التعااملات</t>
   </si>
   <si>
-    <t>DEXAMETHASONE-AMRIYA 8MG/2ML 3 AMP.</t>
-  </si>
-  <si>
-    <t>4:1</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>36.00</t>
-  </si>
-  <si>
-    <t>0:1</t>
-  </si>
-  <si>
-    <t>ETHOXA 250MG/5ML SYRUP 120ML</t>
-  </si>
-  <si>
-    <t>1:0</t>
-  </si>
-  <si>
-    <t>99.00</t>
-  </si>
-  <si>
-    <t>VOLTAREN 75MG/3ML 6 AMP.</t>
-  </si>
-  <si>
-    <t>3:0</t>
-  </si>
-  <si>
-    <t>102.00</t>
-  </si>
-  <si>
-    <t>سرنجات 3 سم</t>
-  </si>
-  <si>
-    <t>0:0</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>2.00</t>
-  </si>
-  <si>
-    <t>سرنجات 5 سم</t>
-  </si>
-  <si>
-    <t>3.00</t>
-  </si>
-  <si>
-    <t>Wednesday, 17 September, 2025 10:47 AM</t>
+    <t>Wednesday, 17 September, 2025 12:45 PM</t>
   </si>
   <si>
     <t>1/1</t>
@@ -314,10 +263,10 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="165" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -326,7 +275,7 @@
     <xf numFmtId="2" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="166" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -732,192 +681,56 @@
     </row>
     <row r="7" ht="25.5" customHeight="1">
       <c r="A7" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B7" s="7"/>
-      <c t="s" r="C7" s="8">
-        <v>10</v>
-      </c>
+      <c r="C7" s="8"/>
       <c r="D7" s="8"/>
       <c r="E7" s="8"/>
       <c r="F7" s="8"/>
       <c r="G7" s="8"/>
-      <c t="s" r="H7" s="9">
-        <v>11</v>
-      </c>
+      <c r="H7" s="9"/>
       <c r="I7" s="9"/>
       <c r="J7" s="9"/>
       <c r="K7" s="9"/>
-      <c t="s" r="L7" s="10">
-        <v>12</v>
-      </c>
+      <c r="L7" s="10"/>
       <c r="M7" s="10"/>
-      <c t="s" r="N7" s="8">
-        <v>13</v>
-      </c>
+      <c r="N7" s="8"/>
       <c r="O7" s="8"/>
       <c r="P7" s="11"/>
-      <c t="s" r="Q7" s="12">
-        <v>14</v>
-      </c>
+      <c r="Q7" s="12"/>
     </row>
     <row r="8" ht="24.75" customHeight="1">
-      <c r="A8" s="7">
-        <v>2</v>
-      </c>
-      <c r="B8" s="7"/>
-      <c t="s" r="C8" s="8">
-        <v>15</v>
-      </c>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c t="s" r="H8" s="9">
-        <v>16</v>
-      </c>
-      <c r="I8" s="9"/>
-      <c r="J8" s="9"/>
-      <c r="K8" s="9"/>
-      <c t="s" r="L8" s="10">
+      <c r="P8" s="13"/>
+      <c r="Q8" s="13"/>
+    </row>
+    <row r="9" ht="16.5" customHeight="1">
+      <c t="s" r="A9" s="14">
+        <v>10</v>
+      </c>
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c t="s" r="G9" s="15">
+        <v>11</v>
+      </c>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="16"/>
+      <c t="s" r="K9" s="17">
         <v>12</v>
       </c>
-      <c r="M8" s="10"/>
-      <c t="s" r="N8" s="8">
-        <v>17</v>
-      </c>
-      <c r="O8" s="8"/>
-      <c r="P8" s="11"/>
-      <c t="s" r="Q8" s="12">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" ht="25.5" customHeight="1">
-      <c r="A9" s="7">
-        <v>3</v>
-      </c>
-      <c r="B9" s="7"/>
-      <c t="s" r="C9" s="8">
-        <v>18</v>
-      </c>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c t="s" r="H9" s="9">
-        <v>19</v>
-      </c>
-      <c r="I9" s="9"/>
-      <c r="J9" s="9"/>
-      <c r="K9" s="9"/>
-      <c t="s" r="L9" s="10">
-        <v>12</v>
-      </c>
-      <c r="M9" s="10"/>
-      <c t="s" r="N9" s="8">
-        <v>20</v>
-      </c>
-      <c r="O9" s="8"/>
-      <c r="P9" s="11"/>
-      <c t="s" r="Q9" s="12">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" ht="24.75" customHeight="1">
-      <c r="A10" s="7">
-        <v>4</v>
-      </c>
-      <c r="B10" s="7"/>
-      <c t="s" r="C10" s="8">
-        <v>21</v>
-      </c>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c t="s" r="H10" s="9">
-        <v>22</v>
-      </c>
-      <c r="I10" s="9"/>
-      <c r="J10" s="9"/>
-      <c r="K10" s="9"/>
-      <c t="s" r="L10" s="10">
-        <v>23</v>
-      </c>
-      <c r="M10" s="10"/>
-      <c t="s" r="N10" s="8">
-        <v>24</v>
-      </c>
-      <c r="O10" s="8"/>
-      <c r="P10" s="11"/>
-      <c t="s" r="Q10" s="12">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" ht="25.5" customHeight="1">
-      <c r="A11" s="7">
-        <v>5</v>
-      </c>
-      <c r="B11" s="7"/>
-      <c t="s" r="C11" s="8">
-        <v>25</v>
-      </c>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c t="s" r="H11" s="9">
-        <v>22</v>
-      </c>
-      <c r="I11" s="9"/>
-      <c r="J11" s="9"/>
-      <c r="K11" s="9"/>
-      <c t="s" r="L11" s="10">
-        <v>23</v>
-      </c>
-      <c r="M11" s="10"/>
-      <c t="s" r="N11" s="8">
-        <v>26</v>
-      </c>
-      <c r="O11" s="8"/>
-      <c r="P11" s="11"/>
-      <c t="s" r="Q11" s="12">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" ht="30" customHeight="1">
-      <c r="P12" s="13">
-        <v>0</v>
-      </c>
-      <c r="Q12" s="13"/>
-    </row>
-    <row r="13" ht="16.5" customHeight="1">
-      <c t="s" r="A13" s="14">
-        <v>27</v>
-      </c>
-      <c r="B13" s="14"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c t="s" r="G13" s="15">
-        <v>28</v>
-      </c>
-      <c r="H13" s="15"/>
-      <c r="I13" s="15"/>
-      <c r="J13" s="16"/>
-      <c t="s" r="K13" s="17">
-        <v>29</v>
-      </c>
-      <c r="L13" s="17"/>
-      <c r="M13" s="17"/>
-      <c r="N13" s="17"/>
-      <c r="O13" s="17"/>
-      <c r="P13" s="17"/>
-      <c r="Q13" s="17"/>
+      <c r="L9" s="17"/>
+      <c r="M9" s="17"/>
+      <c r="N9" s="17"/>
+      <c r="O9" s="17"/>
+      <c r="P9" s="17"/>
+      <c r="Q9" s="17"/>
     </row>
   </sheetData>
-  <mergeCells count="37">
+  <mergeCells count="17">
     <mergeCell ref="D2:N2"/>
     <mergeCell ref="A3:Q3"/>
     <mergeCell ref="F4:H4"/>
@@ -931,30 +744,10 @@
     <mergeCell ref="H7:K7"/>
     <mergeCell ref="L7:M7"/>
     <mergeCell ref="N7:O7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="H8:K8"/>
-    <mergeCell ref="L8:M8"/>
-    <mergeCell ref="N8:O8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="H9:K9"/>
-    <mergeCell ref="L9:M9"/>
-    <mergeCell ref="N9:O9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="H10:K10"/>
-    <mergeCell ref="L10:M10"/>
-    <mergeCell ref="N10:O10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="H11:K11"/>
-    <mergeCell ref="L11:M11"/>
-    <mergeCell ref="N11:O11"/>
-    <mergeCell ref="P12:Q12"/>
-    <mergeCell ref="A13:F13"/>
-    <mergeCell ref="G13:I13"/>
-    <mergeCell ref="K13:Q13"/>
+    <mergeCell ref="P8:Q8"/>
+    <mergeCell ref="A9:F9"/>
+    <mergeCell ref="G9:I9"/>
+    <mergeCell ref="K9:Q9"/>
   </mergeCells>
   <pageMargins left="0.5" right="0.5" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait"/>

</xml_diff>